<commit_message>
Update workbook contents for WUA to AUA change
</commit_message>
<xml_diff>
--- a/RiverArchitect/HabitatEvaluation/.templates/Q_def_hab_template_si.xlsx
+++ b/RiverArchitect/HabitatEvaluation/.templates/Q_def_hab_template_si.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\StreamRestoration\HabitatEvaluation\.templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\RiverArchitect\HabitatEvaluation\.templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,12 +33,6 @@
     <t>Usable Area</t>
   </si>
   <si>
-    <t>WUA</t>
-  </si>
-  <si>
-    <t>Total WUA:</t>
-  </si>
-  <si>
     <t>(filename)</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>(m²/year)</t>
+  </si>
+  <si>
+    <t>AUA</t>
+  </si>
+  <si>
+    <t>Total AUA:</t>
   </si>
 </sst>
 </file>
@@ -927,43 +927,43 @@
         <v>2</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="J2" s="11">
         <f>SUM(G4:G200)</f>
         <v>0</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
@@ -2172,7 +2172,7 @@
     </row>
     <row r="197" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G197" s="16" t="str">
-        <f t="shared" ref="G197:G228" si="6">IF(NOT(ISBLANK(F197)),(E197-E196)/100*F197,"")</f>
+        <f t="shared" ref="G197:G200" si="6">IF(NOT(ISBLANK(F197)),(E197-E196)/100*F197,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>